<commit_message>
added today() function support
</commit_message>
<xml_diff>
--- a/src/test/resources/complex/Complex_template.xlsx
+++ b/src/test/resources/complex/Complex_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeda/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2327F6BA-DD4F-3E48-826B-0480B9C993DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE15B23-ACDD-2A4A-A2AF-B0203E400741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="500" windowWidth="30100" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="30100" windowHeight="17360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>Code</t>
     <phoneticPr fontId="3"/>
@@ -210,9 +210,6 @@
     <t>Record Date</t>
   </si>
   <si>
-    <t>${total(Account Outflow Details:checkInflow)}</t>
-  </si>
-  <si>
     <t>${total(Account Inflow Details:checkInflow)}</t>
   </si>
   <si>
@@ -243,64 +240,70 @@
     <t>${total(NAV Details:clientWithdrawal)}</t>
   </si>
   <si>
-    <t>${colArray(Syntax Report:security_cd)}</t>
-  </si>
-  <si>
-    <t>${colArray(Syntax Report:securityDescription)}</t>
-  </si>
-  <si>
-    <t>${colArray(Syntax Report:market_value_bs)}</t>
-  </si>
-  <si>
-    <t>${colArray(Syntax Report:trade_ccy_cd)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset Outflow Details#assetCode:outflow)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset Outflow Details#assetCode:daysOutflow)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset Inflow Details#assetCode:inflow)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset Inflow Details#assetCode:daysInflow)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset NAV Details:assetCode)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset NAV Details#assetCode:assetName)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset NAV Details#assetCode:previousMonthNAV)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset Inflow Details#assetCode:currentMonthNAV)}</t>
-  </si>
-  <si>
-    <t>${colArray(Asset Inflow Details#assetCode:exposure)}</t>
-  </si>
-  <si>
-    <t>${today(DD/MM/YYYY)}</t>
-  </si>
-  <si>
-    <t>${ref(D21)}</t>
-  </si>
-  <si>
-    <t>${formula(sum(Asset NAV Details#assetCode:previousMonthNAV)}</t>
-  </si>
-  <si>
-    <t>${formula(sum(Asset Inflow Details:exposure)}</t>
-  </si>
-  <si>
-    <t>${formula(sum(Asset Inflow Details:currentMonthNAV)}</t>
-  </si>
-  <si>
-    <t>${formula(sum(Asset Outflow Details:outflow)}</t>
-  </si>
-  <si>
-    <t>${colArr(formula(ref(J14)/ref(J16)))}</t>
+    <t>${row(assetCode#Asset NAV Details:assetCode)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset NAV Details:assetName)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset NAV Details:previousMonthNAV)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset Inflow Details:inflow)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset Inflow Details:daysInflow)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset Outflow Details:outflow)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset Outflow Details:daysOutflow)}</t>
+  </si>
+  <si>
+    <t>${row(security_cd#Syntax Report:securityDescription)}</t>
+  </si>
+  <si>
+    <t>${row(security_cd#Syntax Report:security_cd)}</t>
+  </si>
+  <si>
+    <t>${row(security_cd#Syntax Report:market_value_bs)}</t>
+  </si>
+  <si>
+    <t>${row(security_cd#Syntax Report:trade_ccy_cd)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset NAV Details:currentMonthNAV)}</t>
+  </si>
+  <si>
+    <t>${row(assetCode#Asset NAV Details:exposure)}</t>
+  </si>
+  <si>
+    <t>${ref(14,3)}</t>
+  </si>
+  <si>
+    <t>${totalCol(8,9)}</t>
+  </si>
+  <si>
+    <t>${totalCol(8,8)}</t>
+  </si>
+  <si>
+    <t>${sum(15,3,16,3)}</t>
+  </si>
+  <si>
+    <t>${totalCol(8,3)}</t>
+  </si>
+  <si>
+    <t>${divide(8, 9,9,9)}</t>
+  </si>
+  <si>
+    <t>${totalCol(8,11)}</t>
+  </si>
+  <si>
+    <t>${total(Account Outflow Details:checkOutflow)}</t>
+  </si>
+  <si>
+    <t>${today(dd/MM/YYYY)}</t>
   </si>
 </sst>
 </file>
@@ -1592,6 +1595,60 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1616,9 +1673,6 @@
     <xf numFmtId="38" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1630,57 +1684,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="88">
@@ -2238,8 +2241,8 @@
   </sheetPr>
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2252,7 +2255,7 @@
     <col min="7" max="7" width="58.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="2.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.6640625" style="1" customWidth="1"/>
@@ -2262,17 +2265,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2280,16 +2283,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="84"/>
+      <c r="H3" s="101"/>
       <c r="I3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2307,10 +2310,10 @@
       <c r="F4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="84" t="s">
+      <c r="G4" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="84"/>
+      <c r="H4" s="101"/>
       <c r="I4" s="34" t="s">
         <v>21</v>
       </c>
@@ -2321,18 +2324,18 @@
         <v>33</v>
       </c>
       <c r="D5" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>55</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>56</v>
       </c>
       <c r="F5" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="84" t="s">
+      <c r="G5" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="84"/>
+      <c r="H5" s="101"/>
       <c r="I5" s="34" t="s">
         <v>8</v>
       </c>
@@ -2341,35 +2344,35 @@
     </row>
     <row r="6" spans="2:15" ht="14" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="74"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="78" t="s">
+      <c r="B7" s="92"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73" t="s">
+      <c r="F7" s="91"/>
+      <c r="G7" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="80" t="s">
+      <c r="H7" s="91"/>
+      <c r="I7" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="82" t="s">
+      <c r="J7" s="99" t="s">
         <v>40</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="85" t="s">
+      <c r="L7" s="84" t="s">
         <v>30</v>
       </c>
       <c r="N7" s="62"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="79"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="97"/>
       <c r="E8" s="13" t="s">
         <v>37</v>
       </c>
@@ -2382,26 +2385,26 @@
       <c r="H8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="81"/>
-      <c r="J8" s="83"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="100"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="86"/>
-    </row>
-    <row r="9" spans="2:15" ht="182">
+      <c r="L8" s="85"/>
+    </row>
+    <row r="9" spans="2:15" ht="210">
       <c r="B9" s="46" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F9" s="49" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G9" s="48" t="s">
         <v>65</v>
@@ -2410,17 +2413,17 @@
         <v>66</v>
       </c>
       <c r="I9" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="50" t="s">
-        <v>73</v>
-      </c>
       <c r="L9" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O9" s="31"/>
     </row>
-    <row r="10" spans="2:15" ht="14" thickBot="1">
+    <row r="10" spans="2:15" ht="15" thickBot="1">
       <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
@@ -2428,28 +2431,28 @@
         <v>12</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F10" s="52">
         <v>0</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H10" s="52">
         <v>1</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" s="53">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="L10" s="53" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -2460,69 +2463,69 @@
       <c r="I12" s="33"/>
     </row>
     <row r="14" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="87"/>
+      <c r="C14" s="83"/>
       <c r="I14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="J14" s="65"/>
     </row>
     <row r="15" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="89"/>
+      <c r="C15" s="87"/>
       <c r="D15" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="8"/>
       <c r="I15" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="91"/>
+      <c r="C16" s="89"/>
       <c r="D16" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="8"/>
       <c r="I16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="91"/>
+      <c r="C17" s="89"/>
       <c r="D17" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="29" thickBot="1">
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>15</v>
@@ -2533,28 +2536,28 @@
       <c r="K18" s="64"/>
     </row>
     <row r="21" spans="2:11" ht="14" thickBot="1">
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
     </row>
     <row r="22" spans="2:11" ht="28">
-      <c r="B22" s="98"/>
-      <c r="C22" s="99"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="80" t="s">
+      <c r="E22" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80" t="s">
+      <c r="F22" s="72"/>
+      <c r="G22" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="92"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="68" t="s">
         <v>28</v>
       </c>
@@ -2563,15 +2566,15 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="14" thickBot="1">
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="101"/>
+      <c r="C23" s="82"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
       <c r="I23" s="16">
         <f>E23 - D23</f>
         <v>0</v>
@@ -2587,10 +2590,10 @@
       <c r="J24" s="64"/>
     </row>
     <row r="25" spans="2:11" ht="14" thickBot="1">
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="95"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="19"/>
       <c r="G25" s="28"/>
     </row>
@@ -2620,20 +2623,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
@@ -2644,6 +2633,20 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <printOptions horizontalCentered="1"/>
@@ -2661,8 +2664,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2683,7 +2686,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="63"/>
     </row>
@@ -2701,7 +2704,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C4" s="63"/>
     </row>
@@ -2727,18 +2730,18 @@
     </row>
     <row r="7" spans="1:6" ht="60">
       <c r="A7" s="60" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C7" s="37"/>
       <c r="D7" s="38"/>
       <c r="E7" s="61" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2788,15 +2791,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDC787A71DDF645B3B1EC4B4C087709" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfcc5dabae62faba7569d214b4f3e22c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2910,6 +2904,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
   <ds:schemaRefs>
@@ -2926,14 +2929,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA689A5-2DDE-4193-801A-F36D3E40FA78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2947,4 +2942,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA689A5-2DDE-4193-801A-F36D3E40FA78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding logical stops on delayed rendering
</commit_message>
<xml_diff>
--- a/src/test/resources/complex/Complex_template.xlsx
+++ b/src/test/resources/complex/Complex_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeda/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeda/Documents/json-excel/src/test/resources/complex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE15B23-ACDD-2A4A-A2AF-B0203E400741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162BAA39-1664-F247-B91D-54F32A5C1495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="30100" windowHeight="17360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="640" windowWidth="30100" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
@@ -279,24 +279,15 @@
     <t>${row(assetCode#Asset NAV Details:exposure)}</t>
   </si>
   <si>
-    <t>${ref(14,3)}</t>
-  </si>
-  <si>
     <t>${totalCol(8,9)}</t>
   </si>
   <si>
     <t>${totalCol(8,8)}</t>
   </si>
   <si>
-    <t>${sum(15,3,16,3)}</t>
-  </si>
-  <si>
     <t>${totalCol(8,3)}</t>
   </si>
   <si>
-    <t>${divide(8, 9,9,9)}</t>
-  </si>
-  <si>
     <t>${totalCol(8,11)}</t>
   </si>
   <si>
@@ -304,6 +295,15 @@
   </si>
   <si>
     <t>${today(dd/MM/YYYY)}</t>
+  </si>
+  <si>
+    <t>${ref(16,3)}</t>
+  </si>
+  <si>
+    <t>${sum(16,3,17,3)}</t>
+  </si>
+  <si>
+    <t>${divide(8, 9,11,9)}</t>
   </si>
 </sst>
 </file>
@@ -798,7 +798,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1272,6 +1272,58 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1380,7 +1432,7 @@
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1594,6 +1646,27 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="11" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="11" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2239,10 +2312,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:O33"/>
+  <dimension ref="B2:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2265,17 +2338,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2289,10 +2362,10 @@
         <v>53</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="101" t="s">
+      <c r="G3" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="101"/>
+      <c r="H3" s="108"/>
       <c r="I3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2310,10 +2383,10 @@
       <c r="F4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="101" t="s">
+      <c r="G4" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="101"/>
+      <c r="H4" s="108"/>
       <c r="I4" s="34" t="s">
         <v>21</v>
       </c>
@@ -2332,10 +2405,10 @@
       <c r="F5" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="101" t="s">
+      <c r="G5" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="101"/>
+      <c r="H5" s="108"/>
       <c r="I5" s="34" t="s">
         <v>8</v>
       </c>
@@ -2344,35 +2417,35 @@
     </row>
     <row r="6" spans="2:15" ht="14" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="92"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="96" t="s">
+      <c r="B7" s="99"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91" t="s">
+      <c r="F7" s="98"/>
+      <c r="G7" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="91"/>
-      <c r="I7" s="72" t="s">
+      <c r="H7" s="98"/>
+      <c r="I7" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="99" t="s">
+      <c r="J7" s="106" t="s">
         <v>40</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="91" t="s">
         <v>30</v>
       </c>
       <c r="N7" s="62"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="94"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="97"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="13" t="s">
         <v>37</v>
       </c>
@@ -2385,12 +2458,12 @@
       <c r="H8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="98"/>
-      <c r="J8" s="100"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="107"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="85"/>
-    </row>
-    <row r="9" spans="2:15" ht="210">
+      <c r="L8" s="92"/>
+    </row>
+    <row r="9" spans="2:15" ht="182">
       <c r="B9" s="46" t="s">
         <v>60</v>
       </c>
@@ -2419,188 +2492,208 @@
         <v>72</v>
       </c>
       <c r="L9" s="51" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O9" s="31"/>
     </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:15" s="72" customFormat="1">
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="77"/>
+      <c r="L10" s="78"/>
+      <c r="O10" s="31"/>
+    </row>
+    <row r="11" spans="2:15" s="72" customFormat="1">
+      <c r="B11" s="73"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="77"/>
+      <c r="L11" s="78"/>
+      <c r="O11" s="31"/>
+    </row>
+    <row r="12" spans="2:15" ht="15" thickBot="1">
+      <c r="B12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D12" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="52">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="52">
+        <v>1</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="E14" s="8"/>
+      <c r="I14" s="33"/>
+    </row>
+    <row r="16" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
+      <c r="B16" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="90"/>
+      <c r="I16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="65"/>
+    </row>
+    <row r="17" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B17" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="94"/>
+      <c r="D17" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="I17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B18" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="96"/>
+      <c r="D18" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="I18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="52">
+    </row>
+    <row r="19" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B19" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="96"/>
+      <c r="D19" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="29" thickBot="1">
+      <c r="B20" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="85"/>
+      <c r="D20" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="58">
         <v>0</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="52">
-        <v>1</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="L10" s="53" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15">
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="2:15">
-      <c r="E12" s="8"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="14" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B14" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="83"/>
-      <c r="I14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="65"/>
-    </row>
-    <row r="15" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B15" s="86" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="I15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B16" s="88" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="89"/>
-      <c r="D16" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="I16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B17" s="88" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="89"/>
-      <c r="D17" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="56" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="29" thickBot="1">
-      <c r="B18" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="58">
+      <c r="K20" s="64"/>
+    </row>
+    <row r="23" spans="2:11" ht="14" thickBot="1">
+      <c r="B23" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+    </row>
+    <row r="24" spans="2:11" ht="28">
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="80"/>
+      <c r="I24" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="14" thickBot="1">
+      <c r="B25" s="88" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="89"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="16">
+        <f>E25 - D25</f>
         <v>0</v>
       </c>
-      <c r="K18" s="64"/>
-    </row>
-    <row r="21" spans="2:11" ht="14" thickBot="1">
-      <c r="B21" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-    </row>
-    <row r="22" spans="2:11" ht="28">
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="73"/>
-      <c r="I22" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="69" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="14" thickBot="1">
-      <c r="B23" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="82"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="16">
-        <f>E23 - D23</f>
+      <c r="J25" s="17">
+        <f>I25+G25</f>
         <v>0</v>
       </c>
-      <c r="J23" s="17">
-        <f>I23+G23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="15" thickBot="1">
-      <c r="G24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-    </row>
-    <row r="25" spans="2:11" ht="14" thickBot="1">
-      <c r="B25" s="75" t="s">
+    </row>
+    <row r="26" spans="2:11" ht="15" thickBot="1">
+      <c r="G26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+    </row>
+    <row r="27" spans="2:11" ht="14" thickBot="1">
+      <c r="B27" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="19"/>
-      <c r="G25" s="28"/>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="G26" s="28"/>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="C27" s="83"/>
+      <c r="D27" s="19"/>
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="2:11">
@@ -2613,13 +2706,19 @@
       <c r="G30" s="28"/>
     </row>
     <row r="31" spans="2:11">
-      <c r="G31" s="29"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="2:11">
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="30"/>
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" spans="7:7">
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="7:7">
+      <c r="G35" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -2634,19 +2733,19 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <printOptions horizontalCentered="1"/>
@@ -2664,7 +2763,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2704,7 +2803,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" s="63"/>
     </row>

</xml_diff>